<commit_message>
add style.css file & adjust layout
</commit_message>
<xml_diff>
--- a/static/employee_data.xlsx
+++ b/static/employee_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ4"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,7 +617,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -626,7 +626,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1235</t>
+          <t>3579</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Deputy Director</t>
+          <t>Senior</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -650,61 +650,61 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Y2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA2" t="n">
         <v>4</v>
@@ -716,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="AD2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AE2" t="n">
         <v>3</v>
@@ -729,7 +729,7 @@
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
@@ -739,13 +739,13 @@
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>2025-11-05 03:37:25</t>
+          <t>2025-11-05 03:56:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5543</t>
+          <t>8911</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Senior</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -774,86 +774,86 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>IT Division</t>
+          <t>Brokerage Division</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>4</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q3" t="n">
         <v>1</v>
       </c>
       <c r="R3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T3" t="n">
         <v>5</v>
       </c>
       <c r="U3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="V3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W3" t="n">
         <v>2</v>
       </c>
       <c r="X3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Y3" t="n">
         <v>2</v>
       </c>
       <c r="Z3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AD3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AF3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AG3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
@@ -867,13 +867,13 @@
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>2025-11-05 03:37:25</t>
+          <t>2025-11-05 03:56:54</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -882,7 +882,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2341</t>
+          <t>4567</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -892,110 +892,494 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Deputy Manager</t>
+          <t>Officer</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Network Management Department</t>
+          <t>Brokerage Management Department</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>Brokerage Division</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>4</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>4</v>
+      </c>
+      <c r="R4" t="n">
+        <v>4</v>
+      </c>
+      <c r="S4" t="n">
+        <v>2</v>
+      </c>
+      <c r="T4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U4" t="n">
+        <v>2</v>
+      </c>
+      <c r="V4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" t="n">
+        <v>5</v>
+      </c>
+      <c r="X4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>2025-11-05 03:56:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>294</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5678</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn C</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Senior</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Talent Acquisition</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Human Resources Division</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4</v>
+      </c>
+      <c r="L5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" t="n">
+        <v>3</v>
+      </c>
+      <c r="N5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O5" t="n">
+        <v>5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>4</v>
+      </c>
+      <c r="S5" t="n">
+        <v>3</v>
+      </c>
+      <c r="T5" t="n">
+        <v>3</v>
+      </c>
+      <c r="U5" t="n">
+        <v>4</v>
+      </c>
+      <c r="V5" t="n">
+        <v>4</v>
+      </c>
+      <c r="W5" t="n">
+        <v>3</v>
+      </c>
+      <c r="X5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>2025-11-05 03:55:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>293</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1345</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn B</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Senior</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Brokerage Management Department</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>IT Division</t>
         </is>
       </c>
-      <c r="H4" t="n">
-        <v>3</v>
-      </c>
-      <c r="I4" t="n">
-        <v>4</v>
-      </c>
-      <c r="J4" t="n">
-        <v>3</v>
-      </c>
-      <c r="K4" t="n">
-        <v>4</v>
-      </c>
-      <c r="L4" t="n">
-        <v>3</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2</v>
-      </c>
-      <c r="N4" t="n">
-        <v>4</v>
-      </c>
-      <c r="O4" t="n">
-        <v>2</v>
-      </c>
-      <c r="P4" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>2</v>
-      </c>
-      <c r="R4" t="n">
-        <v>2</v>
-      </c>
-      <c r="S4" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" t="n">
-        <v>4</v>
-      </c>
-      <c r="U4" t="n">
-        <v>5</v>
-      </c>
-      <c r="V4" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" t="n">
-        <v>5</v>
-      </c>
-      <c r="X4" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>5</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH4" t="inlineStr">
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M6" t="n">
+        <v>4</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3</v>
+      </c>
+      <c r="P6" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>4</v>
+      </c>
+      <c r="S6" t="n">
+        <v>5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>5</v>
+      </c>
+      <c r="U6" t="n">
+        <v>5</v>
+      </c>
+      <c r="V6" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" t="n">
+        <v>2</v>
+      </c>
+      <c r="X6" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH6" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="AI4" t="inlineStr">
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>2025-11-05 03:55:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>292</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn A</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Officer</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Brokerage Management Department</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Accounting Division</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="n">
+        <v>5</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>4</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>4</v>
+      </c>
+      <c r="R7" t="n">
+        <v>4</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2</v>
+      </c>
+      <c r="T7" t="n">
+        <v>3</v>
+      </c>
+      <c r="U7" t="n">
+        <v>2</v>
+      </c>
+      <c r="V7" t="n">
+        <v>1</v>
+      </c>
+      <c r="W7" t="n">
+        <v>5</v>
+      </c>
+      <c r="X7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>2025-11-05 03:37:25</t>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>2025-11-05 03:55:04</t>
         </is>
       </c>
     </row>

</xml_diff>